<commit_message>
Revised text in various sections. Added some comments to the code for clarity. Generated the main table variable names table.
</commit_message>
<xml_diff>
--- a/00_raw_data/questionnaire/aD3ds4EVZTq8SfR9dYGqdJ.xlsx
+++ b/00_raw_data/questionnaire/aD3ds4EVZTq8SfR9dYGqdJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e15ef2f1d2299900/Temp/Barbados Fisheries/00_raw_data/questionnaire/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3E789FA-54A6-4E54-B00D-1264944EC7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{A3E789FA-54A6-4E54-B00D-1264944EC7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A7E8541-5C0F-4F65-B753-508D4120D0F7}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14891,9 +14891,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q293"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="30.15234375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A1" t="s">

</xml_diff>